<commit_message>
data change / new graphs
</commit_message>
<xml_diff>
--- a/data/precinct_info.xlsx
+++ b/data/precinct_info.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukekolar/Desktop/mn_poli_research/mpls_2021_election/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826FD099-68EE-554E-9803-86C5AB164C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86ABC900-5A00-364B-8153-D993D1A8F4B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4600" yWindow="680" windowWidth="23800" windowHeight="16940" xr2:uid="{79EF1AFB-4144-AF4F-B1E7-D4182092CF8C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="precincts" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Ward</t>
   </si>
@@ -58,15 +58,6 @@
   </si>
   <si>
     <t>vac_perc_black</t>
-  </si>
-  <si>
-    <t>https://districtr.org/COI/92422</t>
-  </si>
-  <si>
-    <t>https://districtr.org/COI/92537</t>
-  </si>
-  <si>
-    <t>https://districtr.org/COI/92636</t>
   </si>
   <si>
     <t>votes_no</t>
@@ -456,9 +447,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1357CCA-F217-A245-AF47-43375236DADB}">
   <dimension ref="A1:K195"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C66" sqref="C66"/>
+      <selection pane="topRight" activeCell="C144" sqref="C144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -470,7 +461,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -497,10 +488,10 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -2672,7 +2663,7 @@
         <v>7</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D62">
         <v>1380</v>
@@ -2708,7 +2699,7 @@
         <v>7</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D63">
         <v>2060</v>
@@ -2780,7 +2771,7 @@
         <v>7</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D65">
         <v>3410</v>
@@ -5328,26 +5319,15 @@
       </c>
     </row>
     <row r="193" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B193" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="B193" s="1"/>
     </row>
     <row r="194" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B194" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="B194" s="1"/>
     </row>
     <row r="195" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B195" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="B195" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B193" r:id="rId1" xr:uid="{EA7C17D4-39C9-A74B-8655-DB446C07F4D4}"/>
-    <hyperlink ref="B194" r:id="rId2" xr:uid="{C14B00A3-E40A-9B4E-AB40-F42AB65E99EE}"/>
-    <hyperlink ref="B195" r:id="rId3" xr:uid="{4926DB0F-EFF7-9341-80AE-A003BA127AB1}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>